<commit_message>
Correção bug de exibição "Data"
</commit_message>
<xml_diff>
--- a/RDO_modificado.xlsx
+++ b/RDO_modificado.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlosmagno.gomes\OneDrive\Área de Trabalho\System_Developer\RDO_Py_Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlosmagno.gomes\OneDrive\Área de Trabalho\System_Developer\RDO_WebApp_Revisado - Copia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03190E32-DCBA-4D9D-8134-1B80A8A9853F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554C1767-45A4-45EA-BF45-B555244016B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="27-2" sheetId="1" state="hidden" r:id="rId1"/>
@@ -542,7 +542,7 @@
     <numFmt numFmtId="169" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="170" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -762,6 +762,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2164,7 +2172,7 @@
     <xf numFmtId="170" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="170" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="301">
+  <cellXfs count="302">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2779,42 +2787,54 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="30" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="25" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2845,7 +2865,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="30" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2906,6 +2926,9 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="25" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2939,7 +2962,6 @@
     <xf numFmtId="49" fontId="32" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2957,12 +2979,9 @@
     <xf numFmtId="166" fontId="26" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -3700,8 +3719,8 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>87557</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>220907</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>586740</xdr:rowOff>
     </xdr:to>
@@ -8456,8 +8475,8 @@
   </sheetPr>
   <dimension ref="A1:AI69"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="AC14" sqref="AC14"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A11" zoomScale="91" zoomScaleNormal="91" zoomScaleSheetLayoutView="87" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="AE29" sqref="AE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8466,20 +8485,19 @@
     <col min="2" max="2" width="6.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="0.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="4.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="5.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="7.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="4.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="0.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="1.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" style="1" customWidth="1"/>
     <col min="14" max="16" width="4.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="10.85546875" style="1" customWidth="1"/>
     <col min="18" max="18" width="4.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="1.140625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="0.7109375" style="1" customWidth="1"/>
+    <col min="19" max="20" width="4" style="1" customWidth="1"/>
     <col min="21" max="21" width="5.28515625" style="1" customWidth="1"/>
     <col min="22" max="23" width="4.28515625" style="1" customWidth="1"/>
     <col min="24" max="24" width="7" style="1" customWidth="1"/>
@@ -8494,7 +8512,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="276" t="s">
+      <c r="A1" s="281" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="89"/>
@@ -8524,7 +8542,7 @@
       <c r="Z1" s="90"/>
     </row>
     <row r="2" spans="1:29" ht="2.4500000000000002" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="251"/>
+      <c r="A2" s="255"/>
       <c r="B2" s="220"/>
       <c r="C2" s="220"/>
       <c r="D2" s="220"/>
@@ -8552,166 +8570,166 @@
       <c r="Z2" s="221"/>
     </row>
     <row r="3" spans="1:29" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="294" t="s">
+      <c r="A3" s="298" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="73"/>
-      <c r="C3" s="290" t="s">
+      <c r="C3" s="294" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="291"/>
-      <c r="E3" s="291"/>
-      <c r="F3" s="291"/>
-      <c r="G3" s="291"/>
-      <c r="H3" s="291"/>
-      <c r="I3" s="291"/>
-      <c r="J3" s="291"/>
-      <c r="K3" s="291"/>
-      <c r="L3" s="291"/>
-      <c r="M3" s="291"/>
-      <c r="N3" s="291"/>
-      <c r="O3" s="291"/>
-      <c r="P3" s="291"/>
-      <c r="Q3" s="291"/>
-      <c r="R3" s="291"/>
-      <c r="S3" s="291"/>
-      <c r="T3" s="291"/>
-      <c r="U3" s="291"/>
-      <c r="V3" s="292"/>
-      <c r="W3" s="280" t="s">
+      <c r="D3" s="295"/>
+      <c r="E3" s="295"/>
+      <c r="F3" s="295"/>
+      <c r="G3" s="295"/>
+      <c r="H3" s="295"/>
+      <c r="I3" s="295"/>
+      <c r="J3" s="295"/>
+      <c r="K3" s="295"/>
+      <c r="L3" s="295"/>
+      <c r="M3" s="295"/>
+      <c r="N3" s="295"/>
+      <c r="O3" s="295"/>
+      <c r="P3" s="295"/>
+      <c r="Q3" s="295"/>
+      <c r="R3" s="295"/>
+      <c r="S3" s="295"/>
+      <c r="T3" s="295"/>
+      <c r="U3" s="295"/>
+      <c r="V3" s="296"/>
+      <c r="W3" s="285" t="s">
         <v>151</v>
       </c>
       <c r="X3" s="73"/>
-      <c r="Y3" s="288"/>
-      <c r="Z3" s="289"/>
+      <c r="Y3" s="293"/>
+      <c r="Z3" s="248"/>
     </row>
     <row r="4" spans="1:29" ht="3.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="260"/>
-      <c r="B4" s="261"/>
-      <c r="C4" s="261"/>
-      <c r="D4" s="261"/>
-      <c r="E4" s="261"/>
-      <c r="F4" s="261"/>
-      <c r="G4" s="261"/>
-      <c r="H4" s="261"/>
-      <c r="I4" s="261"/>
-      <c r="J4" s="261"/>
-      <c r="K4" s="261"/>
-      <c r="L4" s="261"/>
-      <c r="M4" s="261"/>
-      <c r="N4" s="261"/>
-      <c r="O4" s="261"/>
-      <c r="P4" s="261"/>
-      <c r="Q4" s="261"/>
-      <c r="R4" s="261"/>
-      <c r="S4" s="261"/>
-      <c r="T4" s="261"/>
-      <c r="U4" s="261"/>
-      <c r="V4" s="261"/>
-      <c r="W4" s="261"/>
-      <c r="X4" s="261"/>
-      <c r="Y4" s="261"/>
-      <c r="Z4" s="263"/>
+      <c r="A4" s="264"/>
+      <c r="B4" s="265"/>
+      <c r="C4" s="265"/>
+      <c r="D4" s="265"/>
+      <c r="E4" s="265"/>
+      <c r="F4" s="265"/>
+      <c r="G4" s="265"/>
+      <c r="H4" s="265"/>
+      <c r="I4" s="265"/>
+      <c r="J4" s="265"/>
+      <c r="K4" s="265"/>
+      <c r="L4" s="265"/>
+      <c r="M4" s="265"/>
+      <c r="N4" s="265"/>
+      <c r="O4" s="265"/>
+      <c r="P4" s="265"/>
+      <c r="Q4" s="265"/>
+      <c r="R4" s="265"/>
+      <c r="S4" s="265"/>
+      <c r="T4" s="265"/>
+      <c r="U4" s="265"/>
+      <c r="V4" s="265"/>
+      <c r="W4" s="265"/>
+      <c r="X4" s="265"/>
+      <c r="Y4" s="265"/>
+      <c r="Z4" s="267"/>
     </row>
     <row r="5" spans="1:29" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="287" t="s">
+      <c r="A5" s="292" t="s">
         <v>143</v>
       </c>
       <c r="B5" s="73"/>
-      <c r="C5" s="248"/>
-      <c r="D5" s="246"/>
-      <c r="E5" s="246"/>
-      <c r="F5" s="246"/>
-      <c r="G5" s="246"/>
-      <c r="H5" s="278" t="s">
+      <c r="C5" s="251"/>
+      <c r="D5" s="252"/>
+      <c r="E5" s="252"/>
+      <c r="F5" s="252"/>
+      <c r="G5" s="252"/>
+      <c r="H5" s="283" t="s">
         <v>144</v>
       </c>
       <c r="I5" s="73"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="246"/>
-      <c r="L5" s="246"/>
-      <c r="M5" s="246"/>
-      <c r="N5" s="246"/>
-      <c r="O5" s="246"/>
-      <c r="P5" s="295" t="s">
+      <c r="J5" s="251"/>
+      <c r="K5" s="252"/>
+      <c r="L5" s="252"/>
+      <c r="M5" s="252"/>
+      <c r="N5" s="252"/>
+      <c r="O5" s="252"/>
+      <c r="P5" s="299" t="s">
         <v>145</v>
       </c>
       <c r="Q5" s="73"/>
-      <c r="R5" s="296"/>
-      <c r="S5" s="246"/>
-      <c r="T5" s="246"/>
-      <c r="U5" s="246"/>
-      <c r="V5" s="246"/>
-      <c r="W5" s="246"/>
-      <c r="X5" s="246"/>
-      <c r="Y5" s="246"/>
-      <c r="Z5" s="289"/>
+      <c r="R5" s="300"/>
+      <c r="S5" s="252"/>
+      <c r="T5" s="252"/>
+      <c r="U5" s="252"/>
+      <c r="V5" s="252"/>
+      <c r="W5" s="252"/>
+      <c r="X5" s="252"/>
+      <c r="Y5" s="252"/>
+      <c r="Z5" s="248"/>
     </row>
     <row r="6" spans="1:29" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="112"/>
       <c r="B6" s="73"/>
-      <c r="C6" s="246"/>
-      <c r="D6" s="246"/>
-      <c r="E6" s="246"/>
-      <c r="F6" s="246"/>
-      <c r="G6" s="246"/>
+      <c r="C6" s="252"/>
+      <c r="D6" s="252"/>
+      <c r="E6" s="252"/>
+      <c r="F6" s="252"/>
+      <c r="G6" s="252"/>
       <c r="H6" s="73"/>
-      <c r="I6" s="279"/>
-      <c r="J6" s="246"/>
-      <c r="K6" s="246"/>
-      <c r="L6" s="246"/>
-      <c r="M6" s="246"/>
-      <c r="N6" s="246"/>
-      <c r="O6" s="246"/>
+      <c r="I6" s="284"/>
+      <c r="J6" s="252"/>
+      <c r="K6" s="252"/>
+      <c r="L6" s="252"/>
+      <c r="M6" s="252"/>
+      <c r="N6" s="252"/>
+      <c r="O6" s="252"/>
       <c r="P6" s="73"/>
       <c r="Q6" s="73"/>
-      <c r="R6" s="246"/>
-      <c r="S6" s="246"/>
-      <c r="T6" s="246"/>
-      <c r="U6" s="246"/>
-      <c r="V6" s="246"/>
-      <c r="W6" s="246"/>
-      <c r="X6" s="246"/>
-      <c r="Y6" s="246"/>
-      <c r="Z6" s="289"/>
+      <c r="R6" s="252"/>
+      <c r="S6" s="252"/>
+      <c r="T6" s="252"/>
+      <c r="U6" s="252"/>
+      <c r="V6" s="252"/>
+      <c r="W6" s="252"/>
+      <c r="X6" s="252"/>
+      <c r="Y6" s="252"/>
+      <c r="Z6" s="248"/>
       <c r="AC6" s="62"/>
     </row>
     <row r="7" spans="1:29" ht="5.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="260"/>
-      <c r="B7" s="261"/>
-      <c r="C7" s="262"/>
-      <c r="D7" s="261"/>
-      <c r="E7" s="261"/>
-      <c r="F7" s="261"/>
-      <c r="G7" s="261"/>
-      <c r="H7" s="261"/>
-      <c r="I7" s="261"/>
-      <c r="J7" s="261"/>
-      <c r="K7" s="261"/>
-      <c r="L7" s="261"/>
-      <c r="M7" s="261"/>
-      <c r="N7" s="261"/>
-      <c r="O7" s="261"/>
-      <c r="P7" s="261"/>
-      <c r="Q7" s="261"/>
-      <c r="R7" s="261"/>
-      <c r="S7" s="261"/>
-      <c r="T7" s="261"/>
-      <c r="U7" s="261"/>
-      <c r="V7" s="261"/>
-      <c r="W7" s="261"/>
-      <c r="X7" s="261"/>
-      <c r="Y7" s="261"/>
-      <c r="Z7" s="263"/>
+      <c r="A7" s="264"/>
+      <c r="B7" s="265"/>
+      <c r="C7" s="266"/>
+      <c r="D7" s="265"/>
+      <c r="E7" s="265"/>
+      <c r="F7" s="265"/>
+      <c r="G7" s="265"/>
+      <c r="H7" s="265"/>
+      <c r="I7" s="265"/>
+      <c r="J7" s="265"/>
+      <c r="K7" s="265"/>
+      <c r="L7" s="265"/>
+      <c r="M7" s="265"/>
+      <c r="N7" s="265"/>
+      <c r="O7" s="265"/>
+      <c r="P7" s="265"/>
+      <c r="Q7" s="265"/>
+      <c r="R7" s="265"/>
+      <c r="S7" s="265"/>
+      <c r="T7" s="265"/>
+      <c r="U7" s="265"/>
+      <c r="V7" s="265"/>
+      <c r="W7" s="265"/>
+      <c r="X7" s="265"/>
+      <c r="Y7" s="265"/>
+      <c r="Z7" s="267"/>
     </row>
     <row r="8" spans="1:29" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="182" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="257" t="s">
+      <c r="B8" s="261" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="284"/>
+      <c r="C8" s="289"/>
       <c r="D8" s="76"/>
       <c r="E8" s="76"/>
       <c r="F8" s="76"/>
@@ -8719,7 +8737,7 @@
       <c r="H8" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="257" t="s">
+      <c r="I8" s="261" t="s">
         <v>146</v>
       </c>
       <c r="J8" s="76"/>
@@ -8728,18 +8746,18 @@
       <c r="M8" s="76"/>
       <c r="N8" s="76"/>
       <c r="O8" s="77"/>
-      <c r="P8" s="254" t="s">
+      <c r="P8" s="258" t="s">
         <v>14</v>
       </c>
       <c r="Q8" s="74"/>
-      <c r="R8" s="245"/>
-      <c r="S8" s="246"/>
-      <c r="T8" s="246"/>
-      <c r="U8" s="246"/>
-      <c r="V8" s="246"/>
-      <c r="W8" s="246"/>
+      <c r="R8" s="280"/>
+      <c r="S8" s="252"/>
+      <c r="T8" s="252"/>
+      <c r="U8" s="252"/>
+      <c r="V8" s="252"/>
+      <c r="W8" s="252"/>
       <c r="X8" s="232"/>
-      <c r="Y8" s="285" t="s">
+      <c r="Y8" s="290" t="s">
         <v>15</v>
       </c>
       <c r="Z8" s="94"/>
@@ -8750,31 +8768,31 @@
         <v>12</v>
       </c>
       <c r="C9" s="80"/>
-      <c r="D9" s="293"/>
+      <c r="D9" s="297"/>
       <c r="E9" s="208"/>
       <c r="F9" s="208"/>
       <c r="G9" s="209"/>
       <c r="H9" s="186"/>
-      <c r="I9" s="264" t="s">
+      <c r="I9" s="268" t="s">
         <v>147</v>
       </c>
       <c r="J9" s="79"/>
       <c r="K9" s="79"/>
       <c r="L9" s="79"/>
       <c r="M9" s="80"/>
-      <c r="N9" s="250">
-        <f>D9-R8+1</f>
+      <c r="N9" s="254">
+        <f>R8-D9+1</f>
         <v>1</v>
       </c>
       <c r="O9" s="209"/>
       <c r="P9" s="91"/>
       <c r="Q9" s="74"/>
       <c r="R9" s="247"/>
-      <c r="S9" s="246"/>
-      <c r="T9" s="246"/>
-      <c r="U9" s="246"/>
-      <c r="V9" s="246"/>
-      <c r="W9" s="246"/>
+      <c r="S9" s="252"/>
+      <c r="T9" s="252"/>
+      <c r="U9" s="252"/>
+      <c r="V9" s="252"/>
+      <c r="W9" s="252"/>
       <c r="X9" s="232"/>
       <c r="Y9" s="172">
         <f>N9</f>
@@ -8788,41 +8806,41 @@
         <v>148</v>
       </c>
       <c r="C10" s="71"/>
-      <c r="D10" s="282"/>
-      <c r="E10" s="283"/>
-      <c r="F10" s="283"/>
-      <c r="G10" s="256"/>
+      <c r="D10" s="287"/>
+      <c r="E10" s="288"/>
+      <c r="F10" s="288"/>
+      <c r="G10" s="260"/>
       <c r="H10" s="186"/>
-      <c r="I10" s="281" t="s">
+      <c r="I10" s="286" t="s">
         <v>149</v>
       </c>
       <c r="J10" s="234"/>
       <c r="K10" s="234"/>
       <c r="L10" s="234"/>
       <c r="M10" s="71"/>
-      <c r="N10" s="255">
+      <c r="N10" s="259">
         <f>(D10-D9)-N9+1</f>
         <v>0</v>
       </c>
-      <c r="O10" s="256"/>
+      <c r="O10" s="260"/>
       <c r="P10" s="91"/>
       <c r="Q10" s="74"/>
       <c r="R10" s="247"/>
-      <c r="S10" s="246"/>
-      <c r="T10" s="246"/>
-      <c r="U10" s="246"/>
-      <c r="V10" s="246"/>
-      <c r="W10" s="246"/>
+      <c r="S10" s="252"/>
+      <c r="T10" s="252"/>
+      <c r="U10" s="252"/>
+      <c r="V10" s="252"/>
+      <c r="W10" s="252"/>
       <c r="X10" s="232"/>
       <c r="Y10" s="157"/>
       <c r="Z10" s="158"/>
-      <c r="AB10" s="6">
+      <c r="AB10" s="301">
         <f>WEEKDAY(R8)</f>
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="251" t="s">
+      <c r="A11" s="255" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="220"/>
@@ -8862,7 +8880,7 @@
       <c r="F12" s="76"/>
       <c r="G12" s="76"/>
       <c r="H12" s="77"/>
-      <c r="I12" s="252" t="s">
+      <c r="I12" s="256" t="s">
         <v>21</v>
       </c>
       <c r="J12" s="76"/>
@@ -8952,8 +8970,8 @@
       <c r="V14" s="79"/>
       <c r="W14" s="79"/>
       <c r="X14" s="80"/>
-      <c r="Y14" s="297"/>
-      <c r="Z14" s="298"/>
+      <c r="Y14" s="245"/>
+      <c r="Z14" s="246"/>
     </row>
     <row r="15" spans="1:29" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -8987,7 +9005,7 @@
       <c r="W15" s="79"/>
       <c r="X15" s="80"/>
       <c r="Y15" s="247"/>
-      <c r="Z15" s="289"/>
+      <c r="Z15" s="248"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="60"/>
@@ -9018,11 +9036,11 @@
       <c r="V16" s="234"/>
       <c r="W16" s="234"/>
       <c r="X16" s="71"/>
-      <c r="Y16" s="299"/>
-      <c r="Z16" s="300"/>
+      <c r="Y16" s="249"/>
+      <c r="Z16" s="250"/>
     </row>
     <row r="17" spans="1:35" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="251" t="s">
+      <c r="A17" s="255" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="220"/>
@@ -9052,7 +9070,7 @@
       <c r="Z17" s="221"/>
     </row>
     <row r="18" spans="1:35" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="286" t="s">
+      <c r="A18" s="291" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="76"/>
@@ -9091,7 +9109,7 @@
         <v>41</v>
       </c>
       <c r="U18" s="229"/>
-      <c r="V18" s="253" t="s">
+      <c r="V18" s="257" t="s">
         <v>44</v>
       </c>
       <c r="W18" s="76"/>
@@ -9256,24 +9274,24 @@
       <c r="AD22" s="20"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A23" s="277"/>
+      <c r="A23" s="282"/>
       <c r="B23" s="205"/>
       <c r="C23" s="206"/>
-      <c r="D23" s="249"/>
+      <c r="D23" s="253"/>
       <c r="E23" s="206"/>
       <c r="F23" s="217"/>
       <c r="G23" s="218"/>
       <c r="H23" s="204"/>
       <c r="I23" s="205"/>
       <c r="J23" s="206"/>
-      <c r="K23" s="249"/>
+      <c r="K23" s="253"/>
       <c r="L23" s="206"/>
       <c r="M23" s="217"/>
       <c r="N23" s="218"/>
       <c r="O23" s="230"/>
       <c r="P23" s="205"/>
       <c r="Q23" s="206"/>
-      <c r="R23" s="249"/>
+      <c r="R23" s="253"/>
       <c r="S23" s="206"/>
       <c r="T23" s="217"/>
       <c r="U23" s="218"/>
@@ -9284,7 +9302,7 @@
       <c r="Z23" s="69"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A24" s="265" t="s">
+      <c r="A24" s="269" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="73"/>
@@ -9878,399 +9896,399 @@
       <c r="Z43" s="101"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A44" s="272"/>
-      <c r="B44" s="266"/>
-      <c r="C44" s="266"/>
-      <c r="D44" s="266"/>
-      <c r="E44" s="266"/>
-      <c r="F44" s="266"/>
-      <c r="G44" s="266"/>
-      <c r="H44" s="266"/>
-      <c r="I44" s="266"/>
-      <c r="J44" s="266"/>
-      <c r="K44" s="266"/>
-      <c r="L44" s="266"/>
-      <c r="M44" s="266"/>
-      <c r="N44" s="266"/>
-      <c r="O44" s="266"/>
-      <c r="P44" s="266"/>
-      <c r="Q44" s="266"/>
-      <c r="R44" s="266"/>
-      <c r="S44" s="266"/>
+      <c r="A44" s="276"/>
+      <c r="B44" s="270"/>
+      <c r="C44" s="270"/>
+      <c r="D44" s="270"/>
+      <c r="E44" s="270"/>
+      <c r="F44" s="270"/>
+      <c r="G44" s="270"/>
+      <c r="H44" s="270"/>
+      <c r="I44" s="270"/>
+      <c r="J44" s="270"/>
+      <c r="K44" s="270"/>
+      <c r="L44" s="270"/>
+      <c r="M44" s="270"/>
+      <c r="N44" s="270"/>
+      <c r="O44" s="270"/>
+      <c r="P44" s="270"/>
+      <c r="Q44" s="270"/>
+      <c r="R44" s="270"/>
+      <c r="S44" s="270"/>
       <c r="T44" s="66"/>
-      <c r="U44" s="266"/>
-      <c r="V44" s="266"/>
-      <c r="W44" s="266"/>
-      <c r="X44" s="266"/>
-      <c r="Y44" s="266"/>
-      <c r="Z44" s="267"/>
+      <c r="U44" s="270"/>
+      <c r="V44" s="270"/>
+      <c r="W44" s="270"/>
+      <c r="X44" s="270"/>
+      <c r="Y44" s="270"/>
+      <c r="Z44" s="271"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="273"/>
-      <c r="B45" s="268"/>
-      <c r="C45" s="268"/>
-      <c r="D45" s="268"/>
-      <c r="E45" s="268"/>
-      <c r="F45" s="268"/>
-      <c r="G45" s="268"/>
-      <c r="H45" s="268"/>
-      <c r="I45" s="268"/>
-      <c r="J45" s="268"/>
-      <c r="K45" s="268"/>
-      <c r="L45" s="268"/>
-      <c r="M45" s="268"/>
-      <c r="N45" s="268"/>
-      <c r="O45" s="268"/>
-      <c r="P45" s="268"/>
-      <c r="Q45" s="268"/>
-      <c r="R45" s="268"/>
-      <c r="S45" s="268"/>
+      <c r="A45" s="277"/>
+      <c r="B45" s="272"/>
+      <c r="C45" s="272"/>
+      <c r="D45" s="272"/>
+      <c r="E45" s="272"/>
+      <c r="F45" s="272"/>
+      <c r="G45" s="272"/>
+      <c r="H45" s="272"/>
+      <c r="I45" s="272"/>
+      <c r="J45" s="272"/>
+      <c r="K45" s="272"/>
+      <c r="L45" s="272"/>
+      <c r="M45" s="272"/>
+      <c r="N45" s="272"/>
+      <c r="O45" s="272"/>
+      <c r="P45" s="272"/>
+      <c r="Q45" s="272"/>
+      <c r="R45" s="272"/>
+      <c r="S45" s="272"/>
       <c r="T45" s="68"/>
-      <c r="U45" s="268"/>
-      <c r="V45" s="268"/>
-      <c r="W45" s="268"/>
-      <c r="X45" s="268"/>
-      <c r="Y45" s="268"/>
-      <c r="Z45" s="269"/>
+      <c r="U45" s="272"/>
+      <c r="V45" s="272"/>
+      <c r="W45" s="272"/>
+      <c r="X45" s="272"/>
+      <c r="Y45" s="272"/>
+      <c r="Z45" s="273"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="273"/>
-      <c r="B46" s="268"/>
-      <c r="C46" s="268"/>
-      <c r="D46" s="268"/>
-      <c r="E46" s="268"/>
-      <c r="F46" s="268"/>
-      <c r="G46" s="268"/>
-      <c r="H46" s="268"/>
-      <c r="I46" s="268"/>
-      <c r="J46" s="268"/>
-      <c r="K46" s="268"/>
-      <c r="L46" s="268"/>
-      <c r="M46" s="268"/>
-      <c r="N46" s="268"/>
-      <c r="O46" s="268"/>
-      <c r="P46" s="268"/>
-      <c r="Q46" s="268"/>
-      <c r="R46" s="268"/>
-      <c r="S46" s="268"/>
+      <c r="A46" s="277"/>
+      <c r="B46" s="272"/>
+      <c r="C46" s="272"/>
+      <c r="D46" s="272"/>
+      <c r="E46" s="272"/>
+      <c r="F46" s="272"/>
+      <c r="G46" s="272"/>
+      <c r="H46" s="272"/>
+      <c r="I46" s="272"/>
+      <c r="J46" s="272"/>
+      <c r="K46" s="272"/>
+      <c r="L46" s="272"/>
+      <c r="M46" s="272"/>
+      <c r="N46" s="272"/>
+      <c r="O46" s="272"/>
+      <c r="P46" s="272"/>
+      <c r="Q46" s="272"/>
+      <c r="R46" s="272"/>
+      <c r="S46" s="272"/>
       <c r="T46" s="68"/>
-      <c r="U46" s="268"/>
-      <c r="V46" s="268"/>
-      <c r="W46" s="268"/>
-      <c r="X46" s="268"/>
-      <c r="Y46" s="268"/>
-      <c r="Z46" s="269"/>
+      <c r="U46" s="272"/>
+      <c r="V46" s="272"/>
+      <c r="W46" s="272"/>
+      <c r="X46" s="272"/>
+      <c r="Y46" s="272"/>
+      <c r="Z46" s="273"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="273"/>
-      <c r="B47" s="268"/>
-      <c r="C47" s="268"/>
-      <c r="D47" s="268"/>
-      <c r="E47" s="268"/>
-      <c r="F47" s="268"/>
-      <c r="G47" s="268"/>
-      <c r="H47" s="268"/>
-      <c r="I47" s="268"/>
-      <c r="J47" s="268"/>
-      <c r="K47" s="268"/>
-      <c r="L47" s="268"/>
-      <c r="M47" s="268"/>
-      <c r="N47" s="268"/>
-      <c r="O47" s="268"/>
-      <c r="P47" s="268"/>
-      <c r="Q47" s="268"/>
-      <c r="R47" s="268"/>
-      <c r="S47" s="268"/>
+      <c r="A47" s="277"/>
+      <c r="B47" s="272"/>
+      <c r="C47" s="272"/>
+      <c r="D47" s="272"/>
+      <c r="E47" s="272"/>
+      <c r="F47" s="272"/>
+      <c r="G47" s="272"/>
+      <c r="H47" s="272"/>
+      <c r="I47" s="272"/>
+      <c r="J47" s="272"/>
+      <c r="K47" s="272"/>
+      <c r="L47" s="272"/>
+      <c r="M47" s="272"/>
+      <c r="N47" s="272"/>
+      <c r="O47" s="272"/>
+      <c r="P47" s="272"/>
+      <c r="Q47" s="272"/>
+      <c r="R47" s="272"/>
+      <c r="S47" s="272"/>
       <c r="T47" s="68"/>
-      <c r="U47" s="268"/>
-      <c r="V47" s="268"/>
-      <c r="W47" s="268"/>
-      <c r="X47" s="268"/>
-      <c r="Y47" s="268"/>
-      <c r="Z47" s="269"/>
+      <c r="U47" s="272"/>
+      <c r="V47" s="272"/>
+      <c r="W47" s="272"/>
+      <c r="X47" s="272"/>
+      <c r="Y47" s="272"/>
+      <c r="Z47" s="273"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48" s="273"/>
-      <c r="B48" s="268"/>
-      <c r="C48" s="268"/>
-      <c r="D48" s="268"/>
-      <c r="E48" s="268"/>
-      <c r="F48" s="268"/>
-      <c r="G48" s="268"/>
-      <c r="H48" s="268"/>
-      <c r="I48" s="268"/>
-      <c r="J48" s="268"/>
-      <c r="K48" s="268"/>
-      <c r="L48" s="268"/>
-      <c r="M48" s="268"/>
-      <c r="N48" s="268"/>
-      <c r="O48" s="268"/>
-      <c r="P48" s="268"/>
-      <c r="Q48" s="268"/>
-      <c r="R48" s="268"/>
-      <c r="S48" s="268"/>
+      <c r="A48" s="277"/>
+      <c r="B48" s="272"/>
+      <c r="C48" s="272"/>
+      <c r="D48" s="272"/>
+      <c r="E48" s="272"/>
+      <c r="F48" s="272"/>
+      <c r="G48" s="272"/>
+      <c r="H48" s="272"/>
+      <c r="I48" s="272"/>
+      <c r="J48" s="272"/>
+      <c r="K48" s="272"/>
+      <c r="L48" s="272"/>
+      <c r="M48" s="272"/>
+      <c r="N48" s="272"/>
+      <c r="O48" s="272"/>
+      <c r="P48" s="272"/>
+      <c r="Q48" s="272"/>
+      <c r="R48" s="272"/>
+      <c r="S48" s="272"/>
       <c r="T48" s="68"/>
-      <c r="U48" s="268"/>
-      <c r="V48" s="268"/>
-      <c r="W48" s="268"/>
-      <c r="X48" s="268"/>
-      <c r="Y48" s="268"/>
-      <c r="Z48" s="269"/>
+      <c r="U48" s="272"/>
+      <c r="V48" s="272"/>
+      <c r="W48" s="272"/>
+      <c r="X48" s="272"/>
+      <c r="Y48" s="272"/>
+      <c r="Z48" s="273"/>
     </row>
     <row r="49" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A49" s="273"/>
-      <c r="B49" s="268"/>
-      <c r="C49" s="268"/>
-      <c r="D49" s="268"/>
-      <c r="E49" s="268"/>
-      <c r="F49" s="268"/>
-      <c r="G49" s="268"/>
-      <c r="H49" s="268"/>
-      <c r="I49" s="268"/>
-      <c r="J49" s="268"/>
-      <c r="K49" s="268"/>
-      <c r="L49" s="268"/>
-      <c r="M49" s="268"/>
-      <c r="N49" s="268"/>
-      <c r="O49" s="268"/>
-      <c r="P49" s="268"/>
-      <c r="Q49" s="268"/>
-      <c r="R49" s="268"/>
-      <c r="S49" s="268"/>
+      <c r="A49" s="277"/>
+      <c r="B49" s="272"/>
+      <c r="C49" s="272"/>
+      <c r="D49" s="272"/>
+      <c r="E49" s="272"/>
+      <c r="F49" s="272"/>
+      <c r="G49" s="272"/>
+      <c r="H49" s="272"/>
+      <c r="I49" s="272"/>
+      <c r="J49" s="272"/>
+      <c r="K49" s="272"/>
+      <c r="L49" s="272"/>
+      <c r="M49" s="272"/>
+      <c r="N49" s="272"/>
+      <c r="O49" s="272"/>
+      <c r="P49" s="272"/>
+      <c r="Q49" s="272"/>
+      <c r="R49" s="272"/>
+      <c r="S49" s="272"/>
       <c r="T49" s="68"/>
-      <c r="U49" s="268"/>
-      <c r="V49" s="268"/>
-      <c r="W49" s="268"/>
-      <c r="X49" s="268"/>
-      <c r="Y49" s="268"/>
-      <c r="Z49" s="269"/>
+      <c r="U49" s="272"/>
+      <c r="V49" s="272"/>
+      <c r="W49" s="272"/>
+      <c r="X49" s="272"/>
+      <c r="Y49" s="272"/>
+      <c r="Z49" s="273"/>
       <c r="AC49" s="63" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A50" s="273"/>
-      <c r="B50" s="268"/>
-      <c r="C50" s="268"/>
-      <c r="D50" s="268"/>
-      <c r="E50" s="268"/>
-      <c r="F50" s="268"/>
-      <c r="G50" s="268"/>
-      <c r="H50" s="268"/>
-      <c r="I50" s="268"/>
-      <c r="J50" s="268"/>
-      <c r="K50" s="268"/>
-      <c r="L50" s="268"/>
-      <c r="M50" s="268"/>
-      <c r="N50" s="268"/>
-      <c r="O50" s="268"/>
-      <c r="P50" s="268"/>
-      <c r="Q50" s="268"/>
-      <c r="R50" s="268"/>
-      <c r="S50" s="268"/>
+      <c r="A50" s="277"/>
+      <c r="B50" s="272"/>
+      <c r="C50" s="272"/>
+      <c r="D50" s="272"/>
+      <c r="E50" s="272"/>
+      <c r="F50" s="272"/>
+      <c r="G50" s="272"/>
+      <c r="H50" s="272"/>
+      <c r="I50" s="272"/>
+      <c r="J50" s="272"/>
+      <c r="K50" s="272"/>
+      <c r="L50" s="272"/>
+      <c r="M50" s="272"/>
+      <c r="N50" s="272"/>
+      <c r="O50" s="272"/>
+      <c r="P50" s="272"/>
+      <c r="Q50" s="272"/>
+      <c r="R50" s="272"/>
+      <c r="S50" s="272"/>
       <c r="T50" s="68"/>
-      <c r="U50" s="268"/>
-      <c r="V50" s="268"/>
-      <c r="W50" s="268"/>
-      <c r="X50" s="268"/>
-      <c r="Y50" s="268"/>
-      <c r="Z50" s="269"/>
+      <c r="U50" s="272"/>
+      <c r="V50" s="272"/>
+      <c r="W50" s="272"/>
+      <c r="X50" s="272"/>
+      <c r="Y50" s="272"/>
+      <c r="Z50" s="273"/>
     </row>
     <row r="51" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A51" s="273"/>
-      <c r="B51" s="268"/>
-      <c r="C51" s="268"/>
-      <c r="D51" s="268"/>
-      <c r="E51" s="268"/>
-      <c r="F51" s="268"/>
-      <c r="G51" s="268"/>
-      <c r="H51" s="268"/>
-      <c r="I51" s="268"/>
-      <c r="J51" s="268"/>
-      <c r="K51" s="268"/>
-      <c r="L51" s="268"/>
-      <c r="M51" s="268"/>
-      <c r="N51" s="268"/>
-      <c r="O51" s="268"/>
-      <c r="P51" s="268"/>
-      <c r="Q51" s="268"/>
-      <c r="R51" s="268"/>
-      <c r="S51" s="268"/>
+      <c r="A51" s="277"/>
+      <c r="B51" s="272"/>
+      <c r="C51" s="272"/>
+      <c r="D51" s="272"/>
+      <c r="E51" s="272"/>
+      <c r="F51" s="272"/>
+      <c r="G51" s="272"/>
+      <c r="H51" s="272"/>
+      <c r="I51" s="272"/>
+      <c r="J51" s="272"/>
+      <c r="K51" s="272"/>
+      <c r="L51" s="272"/>
+      <c r="M51" s="272"/>
+      <c r="N51" s="272"/>
+      <c r="O51" s="272"/>
+      <c r="P51" s="272"/>
+      <c r="Q51" s="272"/>
+      <c r="R51" s="272"/>
+      <c r="S51" s="272"/>
       <c r="T51" s="68"/>
-      <c r="U51" s="268"/>
-      <c r="V51" s="268"/>
-      <c r="W51" s="268"/>
-      <c r="X51" s="268"/>
-      <c r="Y51" s="268"/>
-      <c r="Z51" s="269"/>
+      <c r="U51" s="272"/>
+      <c r="V51" s="272"/>
+      <c r="W51" s="272"/>
+      <c r="X51" s="272"/>
+      <c r="Y51" s="272"/>
+      <c r="Z51" s="273"/>
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A52" s="273"/>
-      <c r="B52" s="268"/>
-      <c r="C52" s="268"/>
-      <c r="D52" s="268"/>
-      <c r="E52" s="268"/>
-      <c r="F52" s="268"/>
-      <c r="G52" s="268"/>
-      <c r="H52" s="268"/>
-      <c r="I52" s="268"/>
-      <c r="J52" s="268"/>
-      <c r="K52" s="268"/>
-      <c r="L52" s="268"/>
-      <c r="M52" s="268"/>
-      <c r="N52" s="268"/>
-      <c r="O52" s="268"/>
-      <c r="P52" s="268"/>
-      <c r="Q52" s="268"/>
-      <c r="R52" s="268"/>
-      <c r="S52" s="268"/>
+      <c r="A52" s="277"/>
+      <c r="B52" s="272"/>
+      <c r="C52" s="272"/>
+      <c r="D52" s="272"/>
+      <c r="E52" s="272"/>
+      <c r="F52" s="272"/>
+      <c r="G52" s="272"/>
+      <c r="H52" s="272"/>
+      <c r="I52" s="272"/>
+      <c r="J52" s="272"/>
+      <c r="K52" s="272"/>
+      <c r="L52" s="272"/>
+      <c r="M52" s="272"/>
+      <c r="N52" s="272"/>
+      <c r="O52" s="272"/>
+      <c r="P52" s="272"/>
+      <c r="Q52" s="272"/>
+      <c r="R52" s="272"/>
+      <c r="S52" s="272"/>
       <c r="T52" s="68"/>
-      <c r="U52" s="268"/>
-      <c r="V52" s="268"/>
-      <c r="W52" s="268"/>
-      <c r="X52" s="268"/>
-      <c r="Y52" s="268"/>
-      <c r="Z52" s="269"/>
+      <c r="U52" s="272"/>
+      <c r="V52" s="272"/>
+      <c r="W52" s="272"/>
+      <c r="X52" s="272"/>
+      <c r="Y52" s="272"/>
+      <c r="Z52" s="273"/>
     </row>
     <row r="53" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A53" s="273"/>
-      <c r="B53" s="268"/>
-      <c r="C53" s="268"/>
-      <c r="D53" s="268"/>
-      <c r="E53" s="268"/>
-      <c r="F53" s="268"/>
-      <c r="G53" s="268"/>
-      <c r="H53" s="268"/>
-      <c r="I53" s="268"/>
-      <c r="J53" s="268"/>
-      <c r="K53" s="268"/>
-      <c r="L53" s="268"/>
-      <c r="M53" s="268"/>
-      <c r="N53" s="268"/>
-      <c r="O53" s="268"/>
-      <c r="P53" s="268"/>
-      <c r="Q53" s="268"/>
-      <c r="R53" s="268"/>
-      <c r="S53" s="268"/>
+      <c r="A53" s="277"/>
+      <c r="B53" s="272"/>
+      <c r="C53" s="272"/>
+      <c r="D53" s="272"/>
+      <c r="E53" s="272"/>
+      <c r="F53" s="272"/>
+      <c r="G53" s="272"/>
+      <c r="H53" s="272"/>
+      <c r="I53" s="272"/>
+      <c r="J53" s="272"/>
+      <c r="K53" s="272"/>
+      <c r="L53" s="272"/>
+      <c r="M53" s="272"/>
+      <c r="N53" s="272"/>
+      <c r="O53" s="272"/>
+      <c r="P53" s="272"/>
+      <c r="Q53" s="272"/>
+      <c r="R53" s="272"/>
+      <c r="S53" s="272"/>
       <c r="T53" s="68"/>
-      <c r="U53" s="268"/>
-      <c r="V53" s="268"/>
-      <c r="W53" s="268"/>
-      <c r="X53" s="268"/>
-      <c r="Y53" s="268"/>
-      <c r="Z53" s="269"/>
+      <c r="U53" s="272"/>
+      <c r="V53" s="272"/>
+      <c r="W53" s="272"/>
+      <c r="X53" s="272"/>
+      <c r="Y53" s="272"/>
+      <c r="Z53" s="273"/>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A54" s="273"/>
-      <c r="B54" s="268"/>
-      <c r="C54" s="268"/>
-      <c r="D54" s="268"/>
-      <c r="E54" s="268"/>
-      <c r="F54" s="268"/>
-      <c r="G54" s="268"/>
-      <c r="H54" s="268"/>
-      <c r="I54" s="268"/>
-      <c r="J54" s="268"/>
-      <c r="K54" s="268"/>
-      <c r="L54" s="268"/>
-      <c r="M54" s="268"/>
-      <c r="N54" s="268"/>
-      <c r="O54" s="268"/>
-      <c r="P54" s="268"/>
-      <c r="Q54" s="268"/>
-      <c r="R54" s="268"/>
-      <c r="S54" s="268"/>
+      <c r="A54" s="277"/>
+      <c r="B54" s="272"/>
+      <c r="C54" s="272"/>
+      <c r="D54" s="272"/>
+      <c r="E54" s="272"/>
+      <c r="F54" s="272"/>
+      <c r="G54" s="272"/>
+      <c r="H54" s="272"/>
+      <c r="I54" s="272"/>
+      <c r="J54" s="272"/>
+      <c r="K54" s="272"/>
+      <c r="L54" s="272"/>
+      <c r="M54" s="272"/>
+      <c r="N54" s="272"/>
+      <c r="O54" s="272"/>
+      <c r="P54" s="272"/>
+      <c r="Q54" s="272"/>
+      <c r="R54" s="272"/>
+      <c r="S54" s="272"/>
       <c r="T54" s="68"/>
-      <c r="U54" s="268"/>
-      <c r="V54" s="268"/>
-      <c r="W54" s="268"/>
-      <c r="X54" s="268"/>
-      <c r="Y54" s="268"/>
-      <c r="Z54" s="269"/>
+      <c r="U54" s="272"/>
+      <c r="V54" s="272"/>
+      <c r="W54" s="272"/>
+      <c r="X54" s="272"/>
+      <c r="Y54" s="272"/>
+      <c r="Z54" s="273"/>
     </row>
     <row r="55" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A55" s="273"/>
-      <c r="B55" s="268"/>
-      <c r="C55" s="268"/>
-      <c r="D55" s="268"/>
-      <c r="E55" s="268"/>
-      <c r="F55" s="268"/>
-      <c r="G55" s="268"/>
-      <c r="H55" s="268"/>
-      <c r="I55" s="268"/>
-      <c r="J55" s="268"/>
-      <c r="K55" s="268"/>
-      <c r="L55" s="268"/>
-      <c r="M55" s="268"/>
-      <c r="N55" s="268"/>
-      <c r="O55" s="268"/>
-      <c r="P55" s="268"/>
-      <c r="Q55" s="268"/>
-      <c r="R55" s="268"/>
-      <c r="S55" s="268"/>
+      <c r="A55" s="277"/>
+      <c r="B55" s="272"/>
+      <c r="C55" s="272"/>
+      <c r="D55" s="272"/>
+      <c r="E55" s="272"/>
+      <c r="F55" s="272"/>
+      <c r="G55" s="272"/>
+      <c r="H55" s="272"/>
+      <c r="I55" s="272"/>
+      <c r="J55" s="272"/>
+      <c r="K55" s="272"/>
+      <c r="L55" s="272"/>
+      <c r="M55" s="272"/>
+      <c r="N55" s="272"/>
+      <c r="O55" s="272"/>
+      <c r="P55" s="272"/>
+      <c r="Q55" s="272"/>
+      <c r="R55" s="272"/>
+      <c r="S55" s="272"/>
       <c r="T55" s="68"/>
-      <c r="U55" s="268"/>
-      <c r="V55" s="268"/>
-      <c r="W55" s="268"/>
-      <c r="X55" s="268"/>
-      <c r="Y55" s="268"/>
-      <c r="Z55" s="269"/>
+      <c r="U55" s="272"/>
+      <c r="V55" s="272"/>
+      <c r="W55" s="272"/>
+      <c r="X55" s="272"/>
+      <c r="Y55" s="272"/>
+      <c r="Z55" s="273"/>
     </row>
     <row r="56" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A56" s="273"/>
-      <c r="B56" s="268"/>
-      <c r="C56" s="268"/>
-      <c r="D56" s="268"/>
-      <c r="E56" s="268"/>
-      <c r="F56" s="268"/>
-      <c r="G56" s="268"/>
-      <c r="H56" s="268"/>
-      <c r="I56" s="268"/>
-      <c r="J56" s="268"/>
-      <c r="K56" s="268"/>
-      <c r="L56" s="268"/>
-      <c r="M56" s="268"/>
-      <c r="N56" s="268"/>
-      <c r="O56" s="268"/>
-      <c r="P56" s="268"/>
-      <c r="Q56" s="268"/>
-      <c r="R56" s="268"/>
-      <c r="S56" s="268"/>
+      <c r="A56" s="277"/>
+      <c r="B56" s="272"/>
+      <c r="C56" s="272"/>
+      <c r="D56" s="272"/>
+      <c r="E56" s="272"/>
+      <c r="F56" s="272"/>
+      <c r="G56" s="272"/>
+      <c r="H56" s="272"/>
+      <c r="I56" s="272"/>
+      <c r="J56" s="272"/>
+      <c r="K56" s="272"/>
+      <c r="L56" s="272"/>
+      <c r="M56" s="272"/>
+      <c r="N56" s="272"/>
+      <c r="O56" s="272"/>
+      <c r="P56" s="272"/>
+      <c r="Q56" s="272"/>
+      <c r="R56" s="272"/>
+      <c r="S56" s="272"/>
       <c r="T56" s="68"/>
-      <c r="U56" s="268"/>
-      <c r="V56" s="268"/>
-      <c r="W56" s="268"/>
-      <c r="X56" s="268"/>
-      <c r="Y56" s="268"/>
-      <c r="Z56" s="269"/>
+      <c r="U56" s="272"/>
+      <c r="V56" s="272"/>
+      <c r="W56" s="272"/>
+      <c r="X56" s="272"/>
+      <c r="Y56" s="272"/>
+      <c r="Z56" s="273"/>
     </row>
     <row r="57" spans="1:32" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="273"/>
-      <c r="B57" s="268"/>
-      <c r="C57" s="268"/>
-      <c r="D57" s="268"/>
-      <c r="E57" s="268"/>
-      <c r="F57" s="268"/>
-      <c r="G57" s="268"/>
-      <c r="H57" s="268"/>
-      <c r="I57" s="268"/>
-      <c r="J57" s="268"/>
-      <c r="K57" s="268"/>
-      <c r="L57" s="268"/>
-      <c r="M57" s="268"/>
-      <c r="N57" s="268"/>
-      <c r="O57" s="268"/>
-      <c r="P57" s="268"/>
-      <c r="Q57" s="268"/>
-      <c r="R57" s="268"/>
-      <c r="S57" s="268"/>
+      <c r="A57" s="277"/>
+      <c r="B57" s="272"/>
+      <c r="C57" s="272"/>
+      <c r="D57" s="272"/>
+      <c r="E57" s="272"/>
+      <c r="F57" s="272"/>
+      <c r="G57" s="272"/>
+      <c r="H57" s="272"/>
+      <c r="I57" s="272"/>
+      <c r="J57" s="272"/>
+      <c r="K57" s="272"/>
+      <c r="L57" s="272"/>
+      <c r="M57" s="272"/>
+      <c r="N57" s="272"/>
+      <c r="O57" s="272"/>
+      <c r="P57" s="272"/>
+      <c r="Q57" s="272"/>
+      <c r="R57" s="272"/>
+      <c r="S57" s="272"/>
       <c r="T57" s="68"/>
-      <c r="U57" s="268"/>
-      <c r="V57" s="268"/>
-      <c r="W57" s="268"/>
-      <c r="X57" s="268"/>
-      <c r="Y57" s="268"/>
-      <c r="Z57" s="269"/>
+      <c r="U57" s="272"/>
+      <c r="V57" s="272"/>
+      <c r="W57" s="272"/>
+      <c r="X57" s="272"/>
+      <c r="Y57" s="272"/>
+      <c r="Z57" s="273"/>
       <c r="AA57" s="1"/>
       <c r="AB57" s="1"/>
       <c r="AC57" s="1"/>
@@ -10279,32 +10297,32 @@
       <c r="AF57" s="1"/>
     </row>
     <row r="58" spans="1:32" s="2" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="274"/>
-      <c r="B58" s="270"/>
-      <c r="C58" s="270"/>
-      <c r="D58" s="270"/>
-      <c r="E58" s="270"/>
-      <c r="F58" s="270"/>
-      <c r="G58" s="270"/>
-      <c r="H58" s="270"/>
-      <c r="I58" s="270"/>
-      <c r="J58" s="270"/>
-      <c r="K58" s="270"/>
-      <c r="L58" s="270"/>
-      <c r="M58" s="270"/>
-      <c r="N58" s="270"/>
-      <c r="O58" s="270"/>
-      <c r="P58" s="270"/>
-      <c r="Q58" s="270"/>
-      <c r="R58" s="270"/>
-      <c r="S58" s="270"/>
+      <c r="A58" s="278"/>
+      <c r="B58" s="274"/>
+      <c r="C58" s="274"/>
+      <c r="D58" s="274"/>
+      <c r="E58" s="274"/>
+      <c r="F58" s="274"/>
+      <c r="G58" s="274"/>
+      <c r="H58" s="274"/>
+      <c r="I58" s="274"/>
+      <c r="J58" s="274"/>
+      <c r="K58" s="274"/>
+      <c r="L58" s="274"/>
+      <c r="M58" s="274"/>
+      <c r="N58" s="274"/>
+      <c r="O58" s="274"/>
+      <c r="P58" s="274"/>
+      <c r="Q58" s="274"/>
+      <c r="R58" s="274"/>
+      <c r="S58" s="274"/>
       <c r="T58" s="67"/>
-      <c r="U58" s="270"/>
-      <c r="V58" s="270"/>
-      <c r="W58" s="270"/>
-      <c r="X58" s="270"/>
-      <c r="Y58" s="270"/>
-      <c r="Z58" s="271"/>
+      <c r="U58" s="274"/>
+      <c r="V58" s="274"/>
+      <c r="W58" s="274"/>
+      <c r="X58" s="274"/>
+      <c r="Y58" s="274"/>
+      <c r="Z58" s="275"/>
       <c r="AA58" s="1"/>
       <c r="AB58" s="1"/>
       <c r="AC58" s="1"/>
@@ -10385,7 +10403,7 @@
       </c>
     </row>
     <row r="61" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="259"/>
+      <c r="A61" s="263"/>
       <c r="B61" s="237"/>
       <c r="C61" s="237"/>
       <c r="D61" s="237"/>
@@ -10647,7 +10665,7 @@
       <c r="Z68" s="94"/>
     </row>
     <row r="69" spans="1:32" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="275" t="s">
+      <c r="A69" s="279" t="s">
         <v>150</v>
       </c>
       <c r="B69" s="105"/>
@@ -10663,7 +10681,7 @@
       <c r="L69" s="105"/>
       <c r="M69" s="105"/>
       <c r="N69" s="106"/>
-      <c r="O69" s="258" t="s">
+      <c r="O69" s="262" t="s">
         <v>65</v>
       </c>
       <c r="P69" s="105"/>
@@ -10752,7 +10770,6 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="R8:X10"/>
-    <mergeCell ref="D19:G19"/>
     <mergeCell ref="C5:G6"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="B9:C9"/>
@@ -10810,6 +10827,7 @@
     <mergeCell ref="T23:U23"/>
     <mergeCell ref="A25:Z25"/>
     <mergeCell ref="A59:Z59"/>
+    <mergeCell ref="D19:G19"/>
   </mergeCells>
   <conditionalFormatting sqref="A13:A16">
     <cfRule type="expression" dxfId="4" priority="5">
@@ -10838,7 +10856,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="82" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>